<commit_message>
Esboço da função fight()
</commit_message>
<xml_diff>
--- a/Smoke_Test.xlsx
+++ b/Smoke_Test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t xml:space="preserve">DEFINIÇÕES</t>
   </si>
@@ -461,22 +461,22 @@
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.2755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.8673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="15.8367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="35.8469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="31.6785714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="12.219387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="23.0561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="35.3673469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="11.8061224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="18.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -574,8 +574,8 @@
       <c r="G4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>17</v>
+      <c r="H4" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="I4" s="14" t="s">
         <v>17</v>
@@ -603,8 +603,12 @@
       <c r="G5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="14"/>
+      <c r="H5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="87.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
@@ -616,8 +620,12 @@
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
       <c r="G6" s="17"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="14"/>
+      <c r="H6" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="87.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">

</xml_diff>